<commit_message>
dynamic xls test case file redear with Windows xls file path
</commit_message>
<xml_diff>
--- a/Login Page.xlsx
+++ b/Login Page.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="280">
   <si>
     <t>Signup_Email_GotoProfile</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1960,15 +1960,15 @@
     <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="22.83203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="19.1640625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="13.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="81.0390625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="92.94140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
     <col min="18" max="16384" style="2" width="8.83203125" collapsed="true"/>
   </cols>
@@ -2192,10 +2192,10 @@
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="H5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="I5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J5" t="s">
         <v>274</v>
@@ -2241,10 +2241,10 @@
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="J6" t="s">
         <v>274</v>
@@ -2341,10 +2341,10 @@
       </c>
       <c r="G8" s="28"/>
       <c r="H8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="J8" t="s">
         <v>274</v>
@@ -2392,10 +2392,10 @@
       </c>
       <c r="G9" s="28"/>
       <c r="H9" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I9" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="J9" t="s">
         <v>274</v>
@@ -2441,10 +2441,10 @@
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I10" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="J10" t="s">
         <v>274</v>
@@ -2541,10 +2541,10 @@
       </c>
       <c r="G12" s="28"/>
       <c r="H12" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="I12" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="J12" t="s">
         <v>274</v>
@@ -2784,7 +2784,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="I17" t="s">
         <v>273</v>
@@ -2833,7 +2833,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I18" t="s">
         <v>273</v>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="G20" s="8"/>
       <c r="H20" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I20" t="s">
         <v>273</v>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="G21" s="8"/>
       <c r="H21" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I21" t="s">
         <v>273</v>
@@ -3033,7 +3033,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I22" t="s">
         <v>273</v>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="G24" s="8"/>
       <c r="H24" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="I24" t="s">
         <v>275</v>

</xml_diff>